<commit_message>
Created Mistake Report Folder
Folder that holds the auto generated mistake report that gets referenced from loginBot.py
</commit_message>
<xml_diff>
--- a/Management [DO NOT DELETE].xlsx
+++ b/Management [DO NOT DELETE].xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{86DEB778-8F7E-4EF9-B011-1001D28E0538}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{DE18BFF8-2958-4401-BB2A-6FE69F763231}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E28DEC9-9145-48F2-A114-E68B00D489FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master List" sheetId="1" r:id="rId1"/>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" activeCellId="1" sqref="A1:A1048576 B1:B1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +947,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B7CBDA-FC13-4606-BF9D-97CFCFCDCC6F}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>